<commit_message>
added flask J, K, L; added imgs,
</commit_message>
<xml_diff>
--- a/Analysis/data/metadata/flaskdata.xlsx
+++ b/Analysis/data/metadata/flaskdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmah/Documents/GitHub/Automatic water sampler/Automatic-Water-Sampler/Analysis/metadata/flaskdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmah/Documents/GitHub/Automatic water sampler/Automatic-Water-Sampler/Analysis/data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223AF5B4-A74B-6447-BCBF-5317F0BA748E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E609B1-BDD1-934B-8345-CFB03D4739D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1044,7 +1044,7 @@
   <dimension ref="A1:AO17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1996,10 +1996,10 @@
         <v>8</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G10">
         <v>41</v>
@@ -2008,7 +2008,7 @@
         <v>7</v>
       </c>
       <c r="I10">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="J10" s="2">
         <v>44245</v>
@@ -2071,7 +2071,7 @@
         <v>23</v>
       </c>
       <c r="AD10">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="AE10">
         <v>2</v>
@@ -2106,10 +2106,10 @@
         <v>8</v>
       </c>
       <c r="E11">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G11">
         <v>41</v>
@@ -2118,7 +2118,7 @@
         <v>7</v>
       </c>
       <c r="I11">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="J11" s="2">
         <v>44245</v>
@@ -2216,10 +2216,10 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G12">
         <v>41</v>
@@ -2228,7 +2228,7 @@
         <v>7</v>
       </c>
       <c r="I12">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="J12" s="2">
         <v>44252</v>
@@ -2248,7 +2248,69 @@
       <c r="O12">
         <v>8</v>
       </c>
-      <c r="P12" s="2"/>
+      <c r="P12" s="2">
+        <v>44257</v>
+      </c>
+      <c r="Q12">
+        <v>2021</v>
+      </c>
+      <c r="R12">
+        <v>3</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>8</v>
+      </c>
+      <c r="U12">
+        <v>38</v>
+      </c>
+      <c r="V12">
+        <v>2021</v>
+      </c>
+      <c r="W12">
+        <v>3</v>
+      </c>
+      <c r="X12">
+        <v>2</v>
+      </c>
+      <c r="Y12">
+        <v>15</v>
+      </c>
+      <c r="Z12">
+        <v>45</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>2021</v>
+      </c>
+      <c r="AB12" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="4">
+        <v>23</v>
+      </c>
+      <c r="AE12" s="4">
+        <v>18</v>
+      </c>
+      <c r="AF12" s="4">
+        <v>2021</v>
+      </c>
+      <c r="AG12" s="4">
+        <v>3</v>
+      </c>
+      <c r="AH12" s="4">
+        <v>3</v>
+      </c>
+      <c r="AI12" s="4">
+        <v>8</v>
+      </c>
+      <c r="AJ12" s="4">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -2264,7 +2326,19 @@
         <v>8</v>
       </c>
       <c r="E13">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>19</v>
       </c>
       <c r="J13" s="2">
         <v>44252</v>
@@ -2284,7 +2358,84 @@
       <c r="O13">
         <v>8</v>
       </c>
-      <c r="P13" s="2"/>
+      <c r="P13" s="2">
+        <v>44258</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>2021</v>
+      </c>
+      <c r="R13" s="4">
+        <v>3</v>
+      </c>
+      <c r="S13" s="4">
+        <v>3</v>
+      </c>
+      <c r="T13" s="4">
+        <v>8</v>
+      </c>
+      <c r="U13" s="4">
+        <v>38</v>
+      </c>
+      <c r="V13">
+        <v>2021</v>
+      </c>
+      <c r="W13">
+        <v>3</v>
+      </c>
+      <c r="X13">
+        <v>3</v>
+      </c>
+      <c r="Y13">
+        <v>17</v>
+      </c>
+      <c r="Z13">
+        <v>31</v>
+      </c>
+      <c r="AA13">
+        <v>2021</v>
+      </c>
+      <c r="AB13">
+        <v>3</v>
+      </c>
+      <c r="AC13">
+        <v>3</v>
+      </c>
+      <c r="AD13">
+        <v>19</v>
+      </c>
+      <c r="AE13">
+        <v>38</v>
+      </c>
+      <c r="AF13">
+        <v>2021</v>
+      </c>
+      <c r="AG13">
+        <v>3</v>
+      </c>
+      <c r="AH13">
+        <v>3</v>
+      </c>
+      <c r="AI13">
+        <v>23</v>
+      </c>
+      <c r="AJ13">
+        <v>35</v>
+      </c>
+      <c r="AK13">
+        <v>2021</v>
+      </c>
+      <c r="AL13">
+        <v>3</v>
+      </c>
+      <c r="AM13">
+        <v>4</v>
+      </c>
+      <c r="AN13">
+        <v>9</v>
+      </c>
+      <c r="AO13">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="C14" s="3"/>

</xml_diff>